<commit_message>
moneybin: calculate the smoothing factor (%D)
%D is a simple moving average of %K over a defined smoothing period.

https://investexcel.net/how-to-calculate-the-stochastic-oscillator/

Signed-off-by: Thiago Farina <tfransosi@gmail.com>
</commit_message>
<xml_diff>
--- a/c/apps/moneybin/OSCILLATOR-STOCHASTIC.xlsx
+++ b/c/apps/moneybin/OSCILLATOR-STOCHASTIC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">Stock ticker</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t xml:space="preserve">%K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%D</t>
   </si>
 </sst>
 </file>
@@ -316,14 +319,13 @@
   </sheetPr>
   <dimension ref="A3:B7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8418367346939"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -382,15 +384,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -424,6 +426,9 @@
       <c r="J1" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="K1" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="n">
@@ -792,6 +797,45 @@
       <c r="J16" s="0" t="n">
         <f aca="false">(E16 - I16) / (H16 - I16) * 100</f>
         <v>98.1933526410151</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="n">
+        <v>41407</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>1632.1</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1636</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1626.74</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>1633.77</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>2910600000</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>1633.77</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <f aca="false">MAX(C4:C17)</f>
+        <v>1636</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <f aca="false">MIN(D4:D17)</f>
+        <v>1575.8</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <f aca="false">(E17 - I17) / (H17 - I17) * 100</f>
+        <v>96.2956810631229</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <f aca="false">AVERAGE(J15:J17)</f>
+        <v>94.9609840520359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moneybin: add BPAN4 data to stochastic oscillator spreadsheet
Signed-off-by: Thiago Farina <tfransosi@gmail.com>
</commit_message>
<xml_diff>
--- a/c/apps/moneybin/OSCILLATOR-STOCHASTIC.xlsx
+++ b/c/apps/moneybin/OSCILLATOR-STOCHASTIC.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Data" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="BPAN4" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t xml:space="preserve">Stock ticker</t>
   </si>
@@ -78,10 +79,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D/MMM/YY;@"/>
     <numFmt numFmtId="166" formatCode="M/D/YYYY"/>
+    <numFmt numFmtId="167" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -203,7 +205,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -237,6 +239,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -319,13 +325,15 @@
   </sheetPr>
   <dimension ref="A3:B7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -387,7 +395,479 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.2959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="n">
+        <v>41386</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1555.25</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1565.55</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1548.19</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1562.5</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>2979880000</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1562.5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="n">
+        <v>41387</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1562.5</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1579.58</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1562.5</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1578.78</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>3565150000</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1578.78</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="n">
+        <v>41388</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1578.78</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1583</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1575.8</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1578.79</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>3598240000</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1578.79</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="n">
+        <v>41389</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1578.93</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1592.64</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1578.93</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1585.16</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>3908580000</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>1585.16</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="n">
+        <v>41390</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1585.16</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1585.78</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1577.56</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1582.24</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>3198620000</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>1582.24</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="n">
+        <v>41393</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>1582.34</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1596.65</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1582.34</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1593.61</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>2891200000</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>1593.61</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="n">
+        <v>41394</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1593.58</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1597.57</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1586.5</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1597.57</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>3745070000</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>1597.57</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="n">
+        <v>41395</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>1597.55</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>1597.55</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>1581.28</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1582.7</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>3530320000</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>1582.7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="n">
+        <v>41396</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1582.77</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1598.6</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1582.77</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1597.59</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>3366950000</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>1597.59</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="n">
+        <v>41397</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>1597.6</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1618.46</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>1597.6</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1614.42</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>3603910000</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>1614.42</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="n">
+        <v>41400</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1614.4</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1619.77</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1614.21</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1617.5</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>3062240000</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>1617.5</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="n">
+        <v>41401</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1617.55</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>1626.03</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1616.64</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>1625.96</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>3309580000</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>1625.96</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="n">
+        <v>41402</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>1625.95</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>1632.78</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>1622.7</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>1632.69</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>3554700000</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>1632.69</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="n">
+        <v>41403</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>1632.69</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>1635.01</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>1623.09</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>1626.67</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>3457400000</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>1626.67</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <f aca="false">MAX(Data!C2:C15)</f>
+        <v>1635.01</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <f aca="false">MIN(Data!D2:D15)</f>
+        <v>1548.19</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <f aca="false">(Data!E15 - Data!I15) / (Data!H15 - Data!I15) * 100</f>
+        <v>90.3939184519697</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="n">
+        <v>41404</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>1626.69</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>1633.7</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1623.71</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>1633.7</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>3086470000</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>1633.7</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <f aca="false">MAX(Data!C3:C16)</f>
+        <v>1635.01</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <f aca="false">MIN(Data!D3:D16)</f>
+        <v>1562.5</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <f aca="false">(Data!E16 - Data!I16) / (Data!H16 - Data!I16) * 100</f>
+        <v>98.1933526410151</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="n">
+        <v>41407</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>1632.1</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1636</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1626.74</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>1633.77</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>2910600000</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>1633.77</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <f aca="false">MAX(Data!C4:C17)</f>
+        <v>1636</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <f aca="false">MIN(Data!D4:D17)</f>
+        <v>1575.8</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <f aca="false">(Data!E17 - Data!I17) / (Data!H17 - Data!I17) * 100</f>
+        <v>96.2956810631229</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <f aca="false">AVERAGE(Data!J15:J17)</f>
+        <v>94.9609840520359</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -431,411 +911,411 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="n">
-        <v>41386</v>
+      <c r="A2" s="9" t="n">
+        <v>44308</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1555.25</v>
+        <v>16.16</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1565.55</v>
+        <v>16.290001</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>1548.19</v>
+        <v>14.88</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>1562.5</v>
+        <v>15.11</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>2979880000</v>
+        <v>15.11</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>1562.5</v>
+        <v>9261600</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="n">
-        <v>41387</v>
+      <c r="A3" s="9" t="n">
+        <v>44309</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1562.5</v>
+        <v>15.24</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>1579.58</v>
+        <v>16.690001</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>1562.5</v>
+        <v>15.19</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>1578.78</v>
+        <v>16.360001</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>3565150000</v>
+        <v>16.360001</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>1578.78</v>
+        <v>10938600</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="n">
-        <v>41388</v>
+      <c r="A4" s="9" t="n">
+        <v>44312</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>1578.78</v>
+        <v>16.629999</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>1583</v>
+        <v>17.08</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>1575.8</v>
+        <v>16.4</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>1578.79</v>
+        <v>17</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>3598240000</v>
+        <v>17</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>1578.79</v>
+        <v>9181400</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="n">
-        <v>41389</v>
+      <c r="A5" s="9" t="n">
+        <v>44313</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>1578.93</v>
+        <v>16.950001</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>1592.64</v>
+        <v>18.52</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>1578.93</v>
+        <v>16.799999</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>1585.16</v>
+        <v>17.940001</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>3908580000</v>
+        <v>17.940001</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>1585.16</v>
+        <v>12543800</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="n">
-        <v>41390</v>
+      <c r="A6" s="9" t="n">
+        <v>44314</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>1585.16</v>
+        <v>18.17</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>1585.78</v>
+        <v>18.48</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>1577.56</v>
+        <v>17.41</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>1582.24</v>
+        <v>18.200001</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>3198620000</v>
+        <v>18.200001</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>1582.24</v>
+        <v>6862500</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="n">
-        <v>41393</v>
+      <c r="A7" s="9" t="n">
+        <v>44315</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>1582.34</v>
+        <v>18.209999</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>1596.65</v>
+        <v>19.09</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>1582.34</v>
+        <v>17.620001</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>1593.61</v>
+        <v>17.870001</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>2891200000</v>
+        <v>17.870001</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>1593.61</v>
+        <v>9836600</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="n">
-        <v>41394</v>
+      <c r="A8" s="9" t="n">
+        <v>44316</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>1593.58</v>
+        <v>17.790001</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>1597.57</v>
+        <v>18.5</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>1586.5</v>
+        <v>17.26</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>1597.57</v>
+        <v>18.389999</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>3745070000</v>
+        <v>18.389999</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>1597.57</v>
+        <v>9766900</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="n">
-        <v>41395</v>
+      <c r="A9" s="9" t="n">
+        <v>44319</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>1597.55</v>
+        <v>18.559999</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>1597.55</v>
+        <v>19.25</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>1581.28</v>
+        <v>18.24</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>1582.7</v>
+        <v>18.91</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>3530320000</v>
+        <v>18.902515</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>1582.7</v>
+        <v>7035600</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="n">
-        <v>41396</v>
+      <c r="A10" s="9" t="n">
+        <v>44320</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>1582.77</v>
+        <v>19</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>1598.6</v>
+        <v>19.110001</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>1582.77</v>
+        <v>18.24</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>1597.59</v>
+        <v>18.379999</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>3366950000</v>
+        <v>18.372725</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>1597.59</v>
+        <v>4495700</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="n">
-        <v>41397</v>
+      <c r="A11" s="9" t="n">
+        <v>44321</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>1597.6</v>
+        <v>18.48</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>1618.46</v>
+        <v>19.09</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>1597.6</v>
+        <v>18.120001</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>1614.42</v>
+        <v>19.01</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>3603910000</v>
+        <v>19.01</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>1614.42</v>
+        <v>4288800</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="n">
-        <v>41400</v>
+      <c r="A12" s="9" t="n">
+        <v>44322</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>1614.4</v>
+        <v>18.98</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>1619.77</v>
+        <v>19.49</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>1614.21</v>
+        <v>17.84</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>1617.5</v>
+        <v>18.08</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>3062240000</v>
+        <v>18.08</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>1617.5</v>
+        <v>5505500</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="n">
-        <v>41401</v>
+      <c r="A13" s="9" t="n">
+        <v>44323</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>1617.55</v>
+        <v>18.209999</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>1626.03</v>
+        <v>18.450001</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>1616.64</v>
+        <v>17.9</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>1625.96</v>
+        <v>18.27</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>3309580000</v>
+        <v>18.27</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>1625.96</v>
+        <v>3004200</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="n">
-        <v>41402</v>
+      <c r="A14" s="9" t="n">
+        <v>44326</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>1625.95</v>
+        <v>18.709999</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>1632.78</v>
+        <v>18.92</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>1622.7</v>
+        <v>17.41</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>1632.69</v>
+        <v>17.530001</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>3554700000</v>
+        <v>17.530001</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>1632.69</v>
+        <v>6622000</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="n">
-        <v>41403</v>
+      <c r="A15" s="9" t="n">
+        <v>44327</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>1632.69</v>
+        <v>17.200001</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>1635.01</v>
+        <v>17.459999</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>1623.09</v>
+        <v>16.860001</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>1626.67</v>
+        <v>17.280001</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>3457400000</v>
+        <v>17.280001</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>1626.67</v>
+        <v>3757400</v>
       </c>
       <c r="H15" s="0" t="n">
-        <f aca="false">MAX(C2:C15)</f>
-        <v>1635.01</v>
+        <f aca="false">MAX(BPAN4!C2:C15)</f>
+        <v>19.49</v>
       </c>
       <c r="I15" s="0" t="n">
-        <f aca="false">MIN(D2:D15)</f>
-        <v>1548.19</v>
+        <f aca="false">MIN(BPAN4!D2:D15)</f>
+        <v>14.88</v>
       </c>
       <c r="J15" s="0" t="n">
-        <f aca="false">(E15 - I15) / (H15 - I15) * 100</f>
-        <v>90.3939184519697</v>
+        <f aca="false">(E15-I15) / (H15-I15) * 100</f>
+        <v>52.0607592190889</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="n">
-        <v>41404</v>
+      <c r="A16" s="9" t="n">
+        <v>44328</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>1626.69</v>
+        <v>17.32</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>1633.7</v>
+        <v>17.940001</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>1623.71</v>
+        <v>16.76</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>1633.7</v>
+        <v>16.91</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>3086470000</v>
+        <v>16.91</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>1633.7</v>
+        <v>5068400</v>
       </c>
       <c r="H16" s="0" t="n">
-        <f aca="false">MAX(C3:C16)</f>
-        <v>1635.01</v>
+        <f aca="false">MAX(BPAN4!C3:C16)</f>
+        <v>19.49</v>
       </c>
       <c r="I16" s="0" t="n">
-        <f aca="false">MIN(D3:D16)</f>
-        <v>1562.5</v>
+        <f aca="false">MIN(BPAN4!D3:D16)</f>
+        <v>15.19</v>
       </c>
       <c r="J16" s="0" t="n">
-        <f aca="false">(E16 - I16) / (H16 - I16) * 100</f>
-        <v>98.1933526410151</v>
+        <f aca="false">(E16-I16) / (H16-I16) * 100</f>
+        <v>40</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="n">
-        <v>41407</v>
+      <c r="A17" s="9" t="n">
+        <v>44329</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>1632.1</v>
+        <v>17.1</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>1636</v>
+        <v>18.299999</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>1626.74</v>
+        <v>17</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>1633.77</v>
+        <v>17.870001</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>2910600000</v>
+        <v>17.870001</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>1633.77</v>
+        <v>6646200</v>
       </c>
       <c r="H17" s="0" t="n">
-        <f aca="false">MAX(C4:C17)</f>
-        <v>1636</v>
+        <f aca="false">MAX(BPAN4!C4:C17)</f>
+        <v>19.49</v>
       </c>
       <c r="I17" s="0" t="n">
-        <f aca="false">MIN(D4:D17)</f>
-        <v>1575.8</v>
+        <f aca="false">MIN(BPAN4!D4:D17)</f>
+        <v>16.4</v>
       </c>
       <c r="J17" s="0" t="n">
-        <f aca="false">(E17 - I17) / (H17 - I17) * 100</f>
-        <v>96.2956810631229</v>
+        <f aca="false">(E17-I17) / (H17-I17) * 100</f>
+        <v>47.5728478964401</v>
       </c>
       <c r="K17" s="0" t="n">
         <f aca="false">AVERAGE(J15:J17)</f>
-        <v>94.9609840520359</v>
+        <v>46.5445357051764</v>
       </c>
     </row>
   </sheetData>

</xml_diff>